<commit_message>
Renamed induction to motor.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_ind.xlsx
+++ b/andes/cases/kundur/kundur_ind.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hcui7\repos\andes\andes\cases\kundur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B74387-748D-4C30-9F6B-98B44D87C13E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9229CA5-011F-D94B-9AA2-520764CA8345}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8475" yWindow="1710" windowWidth="28515" windowHeight="15300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34720" yWindow="6400" windowWidth="29480" windowHeight="20540" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="2" r:id="rId1"/>
@@ -834,9 +834,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -880,7 +880,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -924,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -968,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1331,12 +1331,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>100</v>
       </c>
       <c r="G2">
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="H2">
         <v>60</v>
@@ -1480,9 +1480,9 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1562,12 +1562,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1680,9 +1680,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1914,9 +1914,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2048,9 +2048,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2930,7 +2930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3068,9 +3068,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3126,9 +3126,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3560,9 +3560,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3784,9 +3784,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>

</xml_diff>